<commit_message>
creared tables and assumptions
</commit_message>
<xml_diff>
--- a/Output/Table_B.xlsx
+++ b/Output/Table_B.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="122">
   <si>
     <t>model</t>
   </si>
@@ -173,12 +173,21 @@
     <t>39</t>
   </si>
   <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
     <t>a - net chick</t>
   </si>
   <si>
     <t>b - day 14 chick #</t>
   </si>
   <si>
+    <t>c - (a) with sex interaction</t>
+  </si>
+  <si>
     <t>fixed</t>
   </si>
   <si>
@@ -227,6 +236,12 @@
     <t>d14_rear_nest_brood_size</t>
   </si>
   <si>
+    <t>net_rearing_manipulation:chick_sex_molecm</t>
+  </si>
+  <si>
+    <t>net_rearing_manipulation:chick_sex_molecu</t>
+  </si>
+  <si>
     <t>0.037</t>
   </si>
   <si>
@@ -278,48 +293,48 @@
     <t>-0.003</t>
   </si>
   <si>
+    <t>5%</t>
+  </si>
+  <si>
+    <t>0.038</t>
+  </si>
+  <si>
+    <t>37%</t>
+  </si>
+  <si>
+    <t>9%</t>
+  </si>
+  <si>
+    <t>31%</t>
+  </si>
+  <si>
     <t>6%</t>
   </si>
   <si>
-    <t>0.038</t>
-  </si>
-  <si>
-    <t>37%</t>
-  </si>
-  <si>
-    <t>9%</t>
-  </si>
-  <si>
-    <t>31%</t>
+    <t>0.001</t>
   </si>
   <si>
     <t>32%</t>
   </si>
   <si>
+    <t>46%</t>
+  </si>
+  <si>
+    <t>0.041</t>
+  </si>
+  <si>
+    <t>16%</t>
+  </si>
+  <si>
+    <t>4%</t>
+  </si>
+  <si>
+    <t>42%</t>
+  </si>
+  <si>
     <t>11%</t>
   </si>
   <si>
-    <t>5%</t>
-  </si>
-  <si>
-    <t>46%</t>
-  </si>
-  <si>
-    <t>0.041</t>
-  </si>
-  <si>
-    <t>0.001</t>
-  </si>
-  <si>
-    <t>16%</t>
-  </si>
-  <si>
-    <t>4%</t>
-  </si>
-  <si>
-    <t>42%</t>
-  </si>
-  <si>
     <t>2550</t>
   </si>
   <si>
@@ -332,22 +347,37 @@
     <t>-22874.6829362652</t>
   </si>
   <si>
-    <t>0.5</t>
+    <t>-22912.4319348598</t>
+  </si>
+  <si>
+    <t>0.72</t>
+  </si>
+  <si>
+    <t>0.28</t>
   </si>
   <si>
     <t>Inf</t>
   </si>
   <si>
+    <t>2.57</t>
+  </si>
+  <si>
     <t>0.0824199925713075</t>
   </si>
   <si>
     <t>0.0533665666309164</t>
   </si>
   <si>
+    <t>0.0828919527753725</t>
+  </si>
+  <si>
     <t>0.601433846141934</t>
   </si>
   <si>
     <t>0.631831730580635</t>
+  </si>
+  <si>
+    <t>0.602185473025749</t>
   </si>
 </sst>
 </file>
@@ -448,43 +478,43 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="G2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="H2" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="I2" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J2" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
       </c>
       <c r="M2" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="N2" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="O2" t="n">
         <v>0.0</v>
@@ -495,43 +525,43 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F3" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="H3" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I3" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J3" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K3" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L3" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M3" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N3" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O3" t="e">
         <v>#N/A</v>
@@ -542,43 +572,43 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="H4" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I4" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J4" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K4" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L4" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M4" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N4" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O4" t="e">
         <v>#N/A</v>
@@ -589,43 +619,43 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="G5" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="H5" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I5" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J5" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K5" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L5" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M5" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N5" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O5" t="e">
         <v>#N/A</v>
@@ -636,43 +666,43 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F6" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="G6" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="H6" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I6" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J6" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K6" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L6" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M6" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N6" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O6" t="e">
         <v>#N/A</v>
@@ -683,43 +713,43 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E7" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F7" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="G7" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="H7" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I7" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J7" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K7" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L7" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M7" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N7" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O7" t="e">
         <v>#N/A</v>
@@ -730,43 +760,43 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E8" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F8" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="G8" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="H8" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I8" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J8" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K8" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L8" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M8" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N8" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O8" t="e">
         <v>#N/A</v>
@@ -777,43 +807,43 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="F9" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G9" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="H9" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I9" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J9" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K9" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L9" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M9" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N9" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O9" t="e">
         <v>#N/A</v>
@@ -824,43 +854,43 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E10" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F10" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="G10" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="H10" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I10" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J10" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K10" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L10" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M10" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N10" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O10" t="e">
         <v>#N/A</v>
@@ -871,43 +901,43 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F11" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G11" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H11" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I11" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J11" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K11" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L11" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M11" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N11" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O11" t="e">
         <v>#N/A</v>
@@ -918,43 +948,43 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E12" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F12" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H12" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I12" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J12" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K12" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L12" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M12" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N12" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O12" t="e">
         <v>#N/A</v>
@@ -965,43 +995,43 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" t="s">
         <v>80</v>
       </c>
-      <c r="F13" t="s">
-        <v>78</v>
-      </c>
-      <c r="G13" t="s">
-        <v>75</v>
-      </c>
       <c r="H13" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I13" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J13" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K13" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L13" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M13" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N13" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O13" t="e">
         <v>#N/A</v>
@@ -1012,43 +1042,43 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E14" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F14" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="G14" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="H14" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I14" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J14" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K14" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L14" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M14" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N14" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O14" t="e">
         <v>#N/A</v>
@@ -1059,43 +1089,43 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="F15" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="G15" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="H15" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="I15" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="J15" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K15" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="L15" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="M15" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="N15" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="O15" t="n">
         <v>39.59198122120142</v>
@@ -1106,43 +1136,43 @@
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F16" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="G16" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="H16" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I16" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J16" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K16" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L16" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M16" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N16" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O16" t="e">
         <v>#N/A</v>
@@ -1153,43 +1183,43 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F17" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="G17" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="H17" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I17" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J17" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K17" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L17" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M17" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N17" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O17" t="e">
         <v>#N/A</v>
@@ -1200,43 +1230,43 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F18" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="G18" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H18" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I18" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J18" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K18" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L18" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M18" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N18" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O18" t="e">
         <v>#N/A</v>
@@ -1247,43 +1277,43 @@
         <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F19" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="G19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H19" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I19" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J19" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K19" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L19" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M19" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N19" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O19" t="e">
         <v>#N/A</v>
@@ -1294,43 +1324,43 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E20" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F20" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="G20" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="H20" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I20" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J20" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K20" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L20" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M20" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N20" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O20" t="e">
         <v>#N/A</v>
@@ -1341,43 +1371,43 @@
         <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E21" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F21" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="G21" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H21" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I21" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J21" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K21" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L21" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M21" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N21" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O21" t="e">
         <v>#N/A</v>
@@ -1388,43 +1418,43 @@
         <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E22" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F22" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G22" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="H22" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I22" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J22" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K22" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L22" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M22" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N22" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O22" t="e">
         <v>#N/A</v>
@@ -1435,43 +1465,43 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E23" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="F23" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="G23" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="H23" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I23" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J23" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K23" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L23" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M23" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N23" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O23" t="e">
         <v>#N/A</v>
@@ -1482,43 +1512,43 @@
         <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D24" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E24" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F24" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G24" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H24" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I24" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J24" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K24" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L24" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M24" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N24" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O24" t="e">
         <v>#N/A</v>
@@ -1529,43 +1559,43 @@
         <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E25" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F25" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G25" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="H25" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I25" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J25" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K25" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L25" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M25" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N25" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O25" t="e">
         <v>#N/A</v>
@@ -1576,43 +1606,43 @@
         <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C26" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D26" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E26" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F26" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="G26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H26" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I26" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J26" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K26" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L26" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M26" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N26" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O26" t="e">
         <v>#N/A</v>
@@ -1623,43 +1653,43 @@
         <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E27" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F27" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="G27" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="H27" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I27" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J27" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K27" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L27" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M27" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N27" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O27" t="e">
         <v>#N/A</v>
@@ -1670,46 +1700,46 @@
         <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D28" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E28" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F28" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="G28" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="H28" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="I28" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="J28" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K28" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="L28" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
       <c r="M28" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="N28" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="O28" t="n">
-        <v>0.0</v>
+        <v>1.8429826266001328</v>
       </c>
     </row>
     <row r="29">
@@ -1717,43 +1747,43 @@
         <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D29" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E29" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F29" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="G29" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="H29" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I29" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J29" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K29" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L29" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M29" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N29" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O29" t="e">
         <v>#N/A</v>
@@ -1764,43 +1794,43 @@
         <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D30" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E30" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F30" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="G30" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="H30" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I30" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J30" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K30" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L30" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M30" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N30" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O30" t="e">
         <v>#N/A</v>
@@ -1811,43 +1841,43 @@
         <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D31" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E31" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F31" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="G31" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="H31" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I31" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J31" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K31" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L31" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M31" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N31" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O31" t="e">
         <v>#N/A</v>
@@ -1858,43 +1888,43 @@
         <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D32" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E32" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F32" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="G32" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="H32" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I32" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J32" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K32" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L32" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M32" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N32" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O32" t="e">
         <v>#N/A</v>
@@ -1905,43 +1935,43 @@
         <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D33" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="E33" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F33" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G33" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="H33" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I33" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J33" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K33" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L33" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M33" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N33" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O33" t="e">
         <v>#N/A</v>
@@ -1952,43 +1982,43 @@
         <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D34" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="E34" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F34" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G34" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H34" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I34" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J34" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K34" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L34" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M34" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N34" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O34" t="e">
         <v>#N/A</v>
@@ -1999,43 +2029,43 @@
         <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C35" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D35" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E35" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F35" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="G35" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="H35" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I35" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J35" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K35" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L35" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M35" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N35" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O35" t="e">
         <v>#N/A</v>
@@ -2046,43 +2076,43 @@
         <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C36" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D36" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E36" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F36" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="G36" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="H36" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I36" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J36" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K36" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L36" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M36" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N36" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O36" t="e">
         <v>#N/A</v>
@@ -2093,43 +2123,43 @@
         <v>49</v>
       </c>
       <c r="B37" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D37" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E37" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F37" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G37" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H37" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I37" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J37" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K37" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L37" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M37" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N37" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O37" t="e">
         <v>#N/A</v>
@@ -2140,43 +2170,43 @@
         <v>50</v>
       </c>
       <c r="B38" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E38" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F38" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="G38" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="H38" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I38" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J38" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K38" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L38" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M38" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N38" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O38" t="e">
         <v>#N/A</v>
@@ -2187,43 +2217,43 @@
         <v>51</v>
       </c>
       <c r="B39" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C39" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D39" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E39" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F39" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G39" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="H39" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I39" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J39" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K39" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L39" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M39" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N39" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O39" t="e">
         <v>#N/A</v>
@@ -2234,45 +2264,139 @@
         <v>52</v>
       </c>
       <c r="B40" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" t="s">
+        <v>70</v>
+      </c>
+      <c r="E40" t="s">
+        <v>84</v>
+      </c>
+      <c r="F40" t="s">
+        <v>83</v>
+      </c>
+      <c r="G40" t="s">
+        <v>93</v>
+      </c>
+      <c r="H40" t="s">
+        <v>108</v>
+      </c>
+      <c r="I40" t="s">
+        <v>108</v>
+      </c>
+      <c r="J40" t="s">
+        <v>108</v>
+      </c>
+      <c r="K40" t="s">
+        <v>108</v>
+      </c>
+      <c r="L40" t="s">
+        <v>108</v>
+      </c>
+      <c r="M40" t="s">
+        <v>108</v>
+      </c>
+      <c r="N40" t="s">
+        <v>108</v>
+      </c>
+      <c r="O40" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
         <v>53</v>
       </c>
-      <c r="C40" t="s">
-        <v>56</v>
-      </c>
-      <c r="D40" t="s">
-        <v>69</v>
-      </c>
-      <c r="E40" t="s">
-        <v>81</v>
-      </c>
-      <c r="F40" t="s">
+      <c r="B41" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" t="s">
+        <v>71</v>
+      </c>
+      <c r="E41" t="s">
         <v>85</v>
       </c>
-      <c r="G40" t="s">
-        <v>96</v>
-      </c>
-      <c r="H40" t="s">
-        <v>103</v>
-      </c>
-      <c r="I40" t="s">
-        <v>103</v>
-      </c>
-      <c r="J40" t="s">
-        <v>103</v>
-      </c>
-      <c r="K40" t="s">
-        <v>103</v>
-      </c>
-      <c r="L40" t="s">
-        <v>103</v>
-      </c>
-      <c r="M40" t="s">
-        <v>103</v>
-      </c>
-      <c r="N40" t="s">
-        <v>103</v>
-      </c>
-      <c r="O40" t="e">
+      <c r="F41" t="s">
+        <v>83</v>
+      </c>
+      <c r="G41" t="s">
+        <v>80</v>
+      </c>
+      <c r="H41" t="s">
+        <v>108</v>
+      </c>
+      <c r="I41" t="s">
+        <v>108</v>
+      </c>
+      <c r="J41" t="s">
+        <v>108</v>
+      </c>
+      <c r="K41" t="s">
+        <v>108</v>
+      </c>
+      <c r="L41" t="s">
+        <v>108</v>
+      </c>
+      <c r="M41" t="s">
+        <v>108</v>
+      </c>
+      <c r="N41" t="s">
+        <v>108</v>
+      </c>
+      <c r="O41" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" t="s">
+        <v>59</v>
+      </c>
+      <c r="D42" t="s">
+        <v>72</v>
+      </c>
+      <c r="E42" t="s">
+        <v>86</v>
+      </c>
+      <c r="F42" t="s">
+        <v>90</v>
+      </c>
+      <c r="G42" t="s">
+        <v>101</v>
+      </c>
+      <c r="H42" t="s">
+        <v>108</v>
+      </c>
+      <c r="I42" t="s">
+        <v>108</v>
+      </c>
+      <c r="J42" t="s">
+        <v>108</v>
+      </c>
+      <c r="K42" t="s">
+        <v>108</v>
+      </c>
+      <c r="L42" t="s">
+        <v>108</v>
+      </c>
+      <c r="M42" t="s">
+        <v>108</v>
+      </c>
+      <c r="N42" t="s">
+        <v>108</v>
+      </c>
+      <c r="O42" t="e">
         <v>#N/A</v>
       </c>
     </row>

</xml_diff>